<commit_message>
NLP add 2 items Lizuoyan
</commit_message>
<xml_diff>
--- a/NLP_Research.xlsx
+++ b/NLP_Research.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaoxiaoyan/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaoxiaoyan/Desktop/NLP/NIPS_NLP/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>LINK</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,6 +56,51 @@
   </si>
   <si>
     <t>Year</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刘岩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>知乎</t>
+    <rPh sb="0" eb="1">
+      <t>zhi hu</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>csdn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/hengruo/RNet-pytorch/blob/master/models.py</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.Transformer
+2.Self-Attention详细计算</t>
+    <rPh sb="30" eb="31">
+      <t>xiang xi</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>ji suan</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.R-Net py-torch 代码</t>
+    <rPh sb="17" eb="18">
+      <t>dai ma</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hengruo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>github</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -110,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -119,6 +164,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -398,16 +446,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="41.5" style="1" customWidth="1"/>
+    <col min="3" max="5" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -434,13 +483,39 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
-        <v>1</v>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add NLP resources to excel, ivan
</commit_message>
<xml_diff>
--- a/NLP_Research.xlsx
+++ b/NLP_Research.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaoxiaoyan/Desktop/NLP/NIPS_NLP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10426\OneDrive\Documents\assignment2\NIPS_NLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_E5E76EAF6F7C42CF51F5740A3CBE1838DBFF6E88" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5BCBFF42-AA0F-4DF4-8AE6-2C4591E5176A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16720" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>LINK</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -35,11 +36,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://latestainews.blogspot.com/2018/01/r-net.html </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 这篇文章可以理解Enbedding、Attention做了什么事情。
-2.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -103,12 +99,67 @@
     <t>Affiliation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>https://paperswithcode.com/paper/bidirectional-attention-flow-for-machine#code</t>
+  </si>
+  <si>
+    <t>github</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BiDAF Github代码集合</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://zhuanlan.zhihu.com/p/37601161</t>
+  </si>
+  <si>
+    <t>深度学习中的注意力模型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张俊林</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>知乎</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://zhuanlan.zhihu.com/p/49271699</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>word embedding技术的发展历史</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 这篇文章可以理解Embedding、Attention做了什么事情。
+2.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://juditacs.github.io/2018/12/27/masked-attention.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Masking attention weights in PyTorch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>github io</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Judit  Acs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -134,6 +185,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="DengXian"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -152,10 +212,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -169,15 +230,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -445,22 +513,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="41.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="4"/>
-    <col min="4" max="5" width="16.83203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="36.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" style="4"/>
+    <col min="4" max="5" width="16.81640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -468,59 +536,125 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" ht="46.8">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="31.2">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="31.2">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="E4" s="4">
         <v>2018</v>
       </c>
     </row>
+    <row r="5" spans="1:5" ht="31.2">
+      <c r="A5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="4">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="31.2">
+      <c r="A8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2018</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1" location="code" xr:uid="{CCE0022F-9C0C-4F0A-9E0E-9546122EA2E7}"/>
+    <hyperlink ref="A6" r:id="rId2" xr:uid="{046F2041-A977-4B0C-9082-1BA5AB67737E}"/>
+    <hyperlink ref="A7" r:id="rId3" xr:uid="{8B2D3242-225A-479C-8478-98E6AB30A26A}"/>
+    <hyperlink ref="A8" r:id="rId4" xr:uid="{485C55ED-6E3C-429B-BBB8-57FDBE1687F8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>